<commit_message>
add 'created.cdate' in the Select (ref_hps())
</commit_message>
<xml_diff>
--- a/inst/extdata/symbology.xlsx
+++ b/inst/extdata/symbology.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamenaR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Huet\AppData\Local\R\win-library\4.3\eamenaR\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864A68AF-CDA4-4F3A-ACE4-0A5F41FAE67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F05A59-6CF7-4C26-AAE4-DA660447D4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FBCDE9FA-39BE-454A-99C4-DA94C2CE115D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBCDE9FA-39BE-454A-99C4-DA94C2CE115D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Damage Extent Type" sheetId="1" r:id="rId1"/>
+    <sheet name="koppen_climate_class" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>No Visible/Known</t>
   </si>
@@ -62,47 +63,200 @@
     <t>values</t>
   </si>
   <si>
-    <t>colors</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>cat(RColorBrewer::brewer.pal(n = 5, "YlOrRd"), sep = "\n")</t>
-  </si>
-  <si>
-    <t>#FFFFB2</t>
-  </si>
-  <si>
-    <t>#FECC5C</t>
-  </si>
-  <si>
-    <t>#FD8D3C</t>
-  </si>
-  <si>
-    <t>#F03B20</t>
-  </si>
-  <si>
-    <t>#BD0026</t>
-  </si>
-  <si>
-    <t>#808080</t>
-  </si>
-  <si>
-    <t>grey</t>
-  </si>
-  <si>
     <t>list</t>
   </si>
   <si>
     <t>Damage Extent Type</t>
+  </si>
+  <si>
+    <t>FFFFB2</t>
+  </si>
+  <si>
+    <t>FECC5C</t>
+  </si>
+  <si>
+    <t>FD8D3C</t>
+  </si>
+  <si>
+    <t>F03B20</t>
+  </si>
+  <si>
+    <t>BD0026</t>
+  </si>
+  <si>
+    <t>hexa</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Af Tropical, rainforest</t>
+  </si>
+  <si>
+    <t>0000FF</t>
+  </si>
+  <si>
+    <t>Am Tropical, monsoon</t>
+  </si>
+  <si>
+    <t>0078FF</t>
+  </si>
+  <si>
+    <t>Aw Tropical, savannah</t>
+  </si>
+  <si>
+    <t>46AAF</t>
+  </si>
+  <si>
+    <t>BWh Arid, desert, hot</t>
+  </si>
+  <si>
+    <t>FF0000</t>
+  </si>
+  <si>
+    <t>BWk Arid, desert, cold</t>
+  </si>
+  <si>
+    <t>FF9696</t>
+  </si>
+  <si>
+    <t>BSh Arid, steppe, hot</t>
+  </si>
+  <si>
+    <t>F5A500</t>
+  </si>
+  <si>
+    <t>BSk Arid, steppe, cold</t>
+  </si>
+  <si>
+    <t>FFDC64</t>
+  </si>
+  <si>
+    <t>Csa Temperate, dry summer, hot summer</t>
+  </si>
+  <si>
+    <t>FFFF00</t>
+  </si>
+  <si>
+    <t>Csb Temperate, dry summer, warm summer</t>
+  </si>
+  <si>
+    <t>C8C800</t>
+  </si>
+  <si>
+    <t>Csc Temperate, dry summer, cold summer</t>
+  </si>
+  <si>
+    <t>Cwa Temperate, dry winter, hot summer</t>
+  </si>
+  <si>
+    <t>96FF96</t>
+  </si>
+  <si>
+    <t>Cwb Temperate, dry winter, warm summer</t>
+  </si>
+  <si>
+    <t>64C864</t>
+  </si>
+  <si>
+    <t>Cwc Temperate, dry winter, cold summer</t>
+  </si>
+  <si>
+    <t>Cfa Temperate, no dry season, hot summer</t>
+  </si>
+  <si>
+    <t>C8FF50</t>
+  </si>
+  <si>
+    <t>Cfb Temperate, no dry season, warm summer</t>
+  </si>
+  <si>
+    <t>64FF50</t>
+  </si>
+  <si>
+    <t>Cfc Temperate, no dry season, cold summer</t>
+  </si>
+  <si>
+    <t>32C800</t>
+  </si>
+  <si>
+    <t>Dsa Cold, dry summer, hot summer</t>
+  </si>
+  <si>
+    <t>FF00FF</t>
+  </si>
+  <si>
+    <t>Dsb Cold, dry summer, warm summer</t>
+  </si>
+  <si>
+    <t>C800C8</t>
+  </si>
+  <si>
+    <t>Dsc Cold, dry summer, cold summer</t>
+  </si>
+  <si>
+    <t>Dsd Cold, dry summer, very cold winter</t>
+  </si>
+  <si>
+    <t>Dwa Cold, dry winter, hot summer</t>
+  </si>
+  <si>
+    <t>AAAF</t>
+  </si>
+  <si>
+    <t>Dwb Cold, dry winter, warm summer</t>
+  </si>
+  <si>
+    <t>5A78DC</t>
+  </si>
+  <si>
+    <t>Dwc Cold, dry winter, cold summer</t>
+  </si>
+  <si>
+    <t>4B50B4</t>
+  </si>
+  <si>
+    <t>Dwd Cold, dry winter, very cold winter</t>
+  </si>
+  <si>
+    <t>Dfa Cold, no dry season, hot summer</t>
+  </si>
+  <si>
+    <t>00FFFF</t>
+  </si>
+  <si>
+    <t>Dfb Cold, no dry season, warm summer</t>
+  </si>
+  <si>
+    <t>37C8FF</t>
+  </si>
+  <si>
+    <t>Dfc Cold, no dry season, cold summer</t>
+  </si>
+  <si>
+    <t>007D7D</t>
+  </si>
+  <si>
+    <t>Dfd Cold, no dry season, very cold winter</t>
+  </si>
+  <si>
+    <t>00465F</t>
+  </si>
+  <si>
+    <t>ET Polar, tundra</t>
+  </si>
+  <si>
+    <t>B2B2B2</t>
+  </si>
+  <si>
+    <t>EF Polar, frost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +297,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -266,8 +426,9 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="20% - Accent2 2" xfId="6" xr:uid="{299C052B-DE11-41C9-AAB8-F02A9E4A4074}"/>
@@ -603,127 +764,624 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f t="shared" ref="D2:D8" si="0">CONCATENATE("![#",C2,"](https://placehold.co/15x15/",C2,"/",C2,".png)")</f>
+        <v>![#FFFFB2](https://placehold.co/15x15/FFFFB2/FFFFB2.png)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FECC5C](https://placehold.co/15x15/FECC5C/FECC5C.png)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FD8D3C](https://placehold.co/15x15/FD8D3C/FD8D3C.png)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#F03B20](https://placehold.co/15x15/F03B20/F03B20.png)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#BD0026](https://placehold.co/15x15/BD0026/BD0026.png)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>808080</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#808080](https://placehold.co/15x15/808080/808080.png)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>808080</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#808080](https://placehold.co/15x15/808080/808080.png)</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C13:C17">
+    <sortCondition descending="1" ref="C13:C17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41AA9AF-C860-4B23-96DD-2026B42905CA}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
-    <col min="4" max="4" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="1" t="str">
+        <f t="shared" ref="D2:D31" si="0">CONCATENATE("![#",C2,"](https://placehold.co/15x15/",C2,"/",C2,".png)")</f>
+        <v>![#0000FF](https://placehold.co/15x15/0000FF/0000FF.png)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#0078FF](https://placehold.co/15x15/0078FF/0078FF.png)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#46AAF](https://placehold.co/15x15/46AAF/46AAF.png)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FF0000](https://placehold.co/15x15/FF0000/FF0000.png)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FF9696](https://placehold.co/15x15/FF9696/FF9696.png)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#F5A500](https://placehold.co/15x15/F5A500/F5A500.png)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FFDC64](https://placehold.co/15x15/FFDC64/FFDC64.png)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FFFF00](https://placehold.co/15x15/FFFF00/FFFF00.png)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#C8C800](https://placehold.co/15x15/C8C800/C8C800.png)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1">
+        <v>969600</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#969600](https://placehold.co/15x15/969600/969600.png)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#96FF96](https://placehold.co/15x15/96FF96/96FF96.png)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#64C864](https://placehold.co/15x15/64C864/64C864.png)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1">
+        <v>329632</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#329632](https://placehold.co/15x15/329632/329632.png)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#C8FF50](https://placehold.co/15x15/C8FF50/C8FF50.png)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#64FF50](https://placehold.co/15x15/64FF50/64FF50.png)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#32C800](https://placehold.co/15x15/32C800/32C800.png)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#FF00FF](https://placehold.co/15x15/FF00FF/FF00FF.png)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#C800C8](https://placehold.co/15x15/C800C8/C800C8.png)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1">
+        <v>963296</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#963296](https://placehold.co/15x15/963296/963296.png)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1">
+        <v>966496</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#966496](https://placehold.co/15x15/966496/966496.png)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#AAAF](https://placehold.co/15x15/AAAF/AAAF.png)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#5A78DC](https://placehold.co/15x15/5A78DC/5A78DC.png)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#4B50B4](https://placehold.co/15x15/4B50B4/4B50B4.png)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1">
+        <v>320087</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#320087](https://placehold.co/15x15/320087/320087.png)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#00FFFF](https://placehold.co/15x15/00FFFF/00FFFF.png)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#37C8FF](https://placehold.co/15x15/37C8FF/37C8FF.png)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#007D7D](https://placehold.co/15x15/007D7D/007D7D.png)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#00465F](https://placehold.co/15x15/00465F/00465F.png)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#B2B2B2](https://placehold.co/15x15/B2B2B2/B2B2B2.png)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="1">
+        <v>666666</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>![#666666](https://placehold.co/15x15/666666/666666.png)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>